<commit_message>
Konstantencode verbessert zusätzliche Konstanten zum entfernen von 238U von 229Th und 230Th
</commit_message>
<xml_diff>
--- a/data/Yting_260321_20210326-103027/Ratios.xlsx
+++ b/data/Yting_260321_20210326-103027/Ratios.xlsx
@@ -452,7 +452,7 @@
     <col min="18" max="18" width="22.7109375" customWidth="1"/>
     <col min="19" max="19" width="19.7109375" customWidth="1"/>
     <col min="20" max="20" width="23.7109375" customWidth="1"/>
-    <col min="21" max="21" width="19.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -567,22 +567,22 @@
         <v>0.1702428792942349</v>
       </c>
       <c r="P2" s="1">
-        <v>1.318826771892574</v>
+        <v>1.319354151196508</v>
       </c>
       <c r="Q2" s="1">
-        <v>0.5335004453826736</v>
+        <v>0.5343093742747557</v>
       </c>
       <c r="R2" s="1">
-        <v>0.1702371670050599</v>
+        <v>0.1699599420043786</v>
       </c>
       <c r="S2" s="1">
-        <v>1.612895259779135</v>
+        <v>1.613124078274292</v>
       </c>
       <c r="T2" s="1">
-        <v>0.2257985771763353</v>
+        <v>0.2255185977717201</v>
       </c>
       <c r="U2" s="1">
-        <v>1.726512574742643</v>
+        <v>1.726602086087542</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1">
@@ -632,22 +632,22 @@
         <v>0.2105665503060163</v>
       </c>
       <c r="P3" s="2">
-        <v>0.03525043890623247</v>
+        <v>0.03508119734104295</v>
       </c>
       <c r="Q3" s="2">
-        <v>5.705288904693922</v>
+        <v>5.699227156799474</v>
       </c>
       <c r="R3" s="2">
-        <v>0.3294613250209388</v>
+        <v>0.3294025880393198</v>
       </c>
       <c r="S3" s="2">
-        <v>1.213265190703177</v>
+        <v>1.214208209894031</v>
       </c>
       <c r="T3" s="2">
-        <v>0.01157264535611715</v>
+        <v>0.01151406902100858</v>
       </c>
       <c r="U3" s="2">
-        <v>2.453371522281945</v>
+        <v>2.442366103886794</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="1" customFormat="1">
@@ -697,22 +697,22 @@
         <v>0.1328349426970759</v>
       </c>
       <c r="P4" s="1">
-        <v>1.318759177757272</v>
+        <v>1.319295276746676</v>
       </c>
       <c r="Q4" s="1">
-        <v>0.6996313538309004</v>
+        <v>0.700755786729371</v>
       </c>
       <c r="R4" s="1">
-        <v>0.1720259765033036</v>
+        <v>0.1717532801460375</v>
       </c>
       <c r="S4" s="1">
-        <v>1.288866266384345</v>
+        <v>1.289720296490281</v>
       </c>
       <c r="T4" s="1">
-        <v>0.2271470050020687</v>
+        <v>0.2268636021468044</v>
       </c>
       <c r="U4" s="1">
-        <v>1.004207089032775</v>
+        <v>1.004357317888425</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1">
@@ -762,22 +762,22 @@
         <v>0.5107608796364961</v>
       </c>
       <c r="P5" s="2">
-        <v>0.005921825770778144</v>
+        <v>0.005800569700777472</v>
       </c>
       <c r="Q5" s="2">
-        <v>2.813032265449945</v>
+        <v>2.870256697228719</v>
       </c>
       <c r="R5" s="2">
-        <v>0.2259939097674143</v>
+        <v>0.225966131783047</v>
       </c>
       <c r="S5" s="2">
-        <v>1.381875981856847</v>
+        <v>1.381881207195067</v>
       </c>
       <c r="T5" s="2">
-        <v>0.001274691673562648</v>
+        <v>0.001249788646980554</v>
       </c>
       <c r="U5" s="2">
-        <v>2.97747271498213</v>
+        <v>3.023219177889351</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="1" customFormat="1">
@@ -827,22 +827,22 @@
         <v>0.1429583220526351</v>
       </c>
       <c r="P6" s="1">
-        <v>1.313374031600917</v>
+        <v>1.313872396141101</v>
       </c>
       <c r="Q6" s="1">
-        <v>0.5419107723895897</v>
+        <v>0.5427985995815223</v>
       </c>
       <c r="R6" s="1">
-        <v>0.1815114725115821</v>
+        <v>0.181231969044914</v>
       </c>
       <c r="S6" s="1">
-        <v>1.276965247862709</v>
+        <v>1.277445604693938</v>
       </c>
       <c r="T6" s="1">
-        <v>0.2393293430170869</v>
+        <v>0.2390518927769061</v>
       </c>
       <c r="U6" s="1">
-        <v>1.28265146190901</v>
+        <v>1.282867073244825</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="2" customFormat="1">
@@ -892,22 +892,22 @@
         <v>0.1960179186031242</v>
       </c>
       <c r="P7" s="2">
-        <v>0.01783305396177997</v>
+        <v>0.01772214606612332</v>
       </c>
       <c r="Q7" s="2">
-        <v>1.001748480524192</v>
+        <v>1.007265011142688</v>
       </c>
       <c r="R7" s="2">
-        <v>0.249544100283467</v>
+        <v>0.249516127586646</v>
       </c>
       <c r="S7" s="2">
-        <v>0.5610059207786317</v>
+        <v>0.5610571919223687</v>
       </c>
       <c r="T7" s="2">
-        <v>0.004458367135931112</v>
+        <v>0.004430472498451357</v>
       </c>
       <c r="U7" s="2">
-        <v>0.6951876357866389</v>
+        <v>0.6991204502526103</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="1" customFormat="1">
@@ -957,22 +957,22 @@
         <v>0.1455035210538751</v>
       </c>
       <c r="P8" s="1">
-        <v>1.313892579368417</v>
+        <v>1.31437756824995</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.4004394967171863</v>
+        <v>0.4010354484850985</v>
       </c>
       <c r="R8" s="1">
-        <v>0.1792768137488384</v>
+        <v>0.1790024332032209</v>
       </c>
       <c r="S8" s="1">
-        <v>1.36931034548719</v>
+        <v>1.369577648543971</v>
       </c>
       <c r="T8" s="1">
-        <v>0.2374191339979786</v>
+        <v>0.237144123290771</v>
       </c>
       <c r="U8" s="1">
-        <v>1.300845587375957</v>
+        <v>1.300904984569476</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="2" customFormat="1">
@@ -1022,22 +1022,22 @@
         <v>0.1598112027448663</v>
       </c>
       <c r="P9" s="2">
-        <v>0.1438931916272418</v>
+        <v>0.1435039070995674</v>
       </c>
       <c r="Q9" s="2">
-        <v>0.365815313729743</v>
+        <v>0.3667519741005789</v>
       </c>
       <c r="R9" s="2">
-        <v>0.01854280137926809</v>
+        <v>0.01853434975554646</v>
       </c>
       <c r="S9" s="2">
-        <v>0.2678043872163008</v>
+        <v>0.2678958047286344</v>
       </c>
       <c r="T9" s="2">
-        <v>0.002664781889775179</v>
+        <v>0.002656456282872149</v>
       </c>
       <c r="U9" s="2">
-        <v>0.3003130595442578</v>
+        <v>0.3014671536941368</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1">
@@ -1087,22 +1087,22 @@
         <v>0.1329589028485957</v>
       </c>
       <c r="P10" s="1">
-        <v>1.312935307459668</v>
+        <v>1.313423515094221</v>
       </c>
       <c r="Q10" s="1">
-        <v>0.5991393735161512</v>
+        <v>0.6000345397267552</v>
       </c>
       <c r="R10" s="1">
-        <v>0.1781077787529703</v>
+        <v>0.1778374152229192</v>
       </c>
       <c r="S10" s="1">
-        <v>1.347426895188685</v>
+        <v>1.347700761114009</v>
       </c>
       <c r="T10" s="1">
-        <v>0.2340798179609642</v>
+        <v>0.2338113376116541</v>
       </c>
       <c r="U10" s="1">
-        <v>1.249551913334694</v>
+        <v>1.249485075210555</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="2" customFormat="1">
@@ -1152,22 +1152,22 @@
         <v>0.1181142656994044</v>
       </c>
       <c r="P11" s="2">
-        <v>0.1434984853044898</v>
+        <v>0.1431288548060866</v>
       </c>
       <c r="Q11" s="2">
-        <v>0.3364171721037157</v>
+        <v>0.3371065744325605</v>
       </c>
       <c r="R11" s="2">
-        <v>0.0009631928586580701</v>
+        <v>0.0009627681596341573</v>
       </c>
       <c r="S11" s="2">
-        <v>0.255338915736973</v>
+        <v>0.2554890408774075</v>
       </c>
       <c r="T11" s="2">
-        <v>0.0001387130736508046</v>
+        <v>0.0001382911205746749</v>
       </c>
       <c r="U11" s="2">
-        <v>0.2564753741715639</v>
+        <v>0.2574720496270163</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="1" customFormat="1">
@@ -1217,22 +1217,22 @@
         <v>0.1354055892860333</v>
       </c>
       <c r="P12" s="1">
-        <v>1.318059551970325</v>
+        <v>1.318565502507402</v>
       </c>
       <c r="Q12" s="1">
-        <v>0.4537665522382115</v>
+        <v>0.4544712691125686</v>
       </c>
       <c r="R12" s="1">
-        <v>0.1784094620679704</v>
+        <v>0.1781347151424396</v>
       </c>
       <c r="S12" s="1">
-        <v>1.295662586723902</v>
+        <v>1.295526126832855</v>
       </c>
       <c r="T12" s="1">
-        <v>0.2343682381076229</v>
+        <v>0.2340996154520834</v>
       </c>
       <c r="U12" s="1">
-        <v>1.283193429135786</v>
+        <v>1.282918122977668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>